<commit_message>
Jira Defect TestData and Exception Details Added. DryRun Works Fine.
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/AddTaskTestData.xlsx
+++ b/src/test/resources/testData/AddTaskTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Intellij_Env\WebAppTestFramework\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8183AB-F694-4A76-86A5-87DF73DC33D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887FFEBE-C48A-4C83-B98E-72E937005510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5F7D3B99-D034-441B-B1F7-06ED4F3CD305}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Sr No</t>
   </si>
@@ -57,39 +57,18 @@
     <t>CreateTask with Open Status</t>
   </si>
   <si>
-    <t>Create Defect wtith Reopen Status</t>
-  </si>
-  <si>
     <t>Change Priority Rate (Hourly rate $25.00)</t>
   </si>
   <si>
-    <t>Defects (Hourly rate $0.00)</t>
-  </si>
-  <si>
     <t>Open</t>
   </si>
   <si>
-    <t>Re-opened</t>
-  </si>
-  <si>
     <t>Task</t>
   </si>
   <si>
-    <t>Bug</t>
-  </si>
-  <si>
-    <t>Urgent</t>
-  </si>
-  <si>
     <t>Test1</t>
   </si>
   <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>2024-02-24</t>
-  </si>
-  <si>
     <t>2024-02-29</t>
   </si>
   <si>
@@ -108,9 +87,6 @@
     <t>Test Project1</t>
   </si>
   <si>
-    <t>Test Project2</t>
-  </si>
-  <si>
     <t>TaskLabel</t>
   </si>
   <si>
@@ -142,6 +118,9 @@
   </si>
   <si>
     <t>John</t>
+  </si>
+  <si>
+    <t>2024-02-27</t>
   </si>
 </sst>
 </file>
@@ -215,7 +194,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -223,7 +202,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -539,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3FA0CC-B4DB-4341-A9AD-E7F79838C2AC}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,7 +560,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>5</v>
@@ -597,28 +575,28 @@
         <v>8</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="M1" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -630,111 +608,56 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="K2" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="4">
+        <v>2</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>5</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="N2" s="4">
-        <v>5</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2" s="7">
-        <v>5</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="4">
-        <v>5</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q3" s="7">
-        <v>95</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{98A8D6AD-B550-40B1-A0CD-C064FB42FF64}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{BCE98420-31B3-41FA-BAC4-C0A7F3BDFC69}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>